<commit_message>
se crea el archivo ocupacionPuertos y se completa los casos de prueba gestionCambioNapPuerto
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestionCambioNapPuerto.page.xlsx
+++ b/docs/test-cases/gestionCambioNapPuerto.page.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DE88C2-069C-4196-9D58-A0B987BE54B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gestionCambioNapPuerto" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>ID Caso</t>
   </si>
@@ -90,13 +91,57 @@
   </si>
   <si>
     <t>El sistema debe redirigido correctamente la vista Gestión cambio de nap y puerto</t>
+  </si>
+  <si>
+    <t>CP_GESCAMNAPPUER_002</t>
+  </si>
+  <si>
+    <t>Seleccionar una nap</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Clic en el botón Picklist
+2. Diligenciar campo "Buscar" con la NAP
+3. Seleccionar el registro de la NAP
+4.Clic en el botón "Seleccionar" del modal
+</t>
+  </si>
+  <si>
+    <t>El sistema debe seleccionado una nap correctamente</t>
+  </si>
+  <si>
+    <t>se selecciono la nap correctamente</t>
+  </si>
+  <si>
+    <t>CP_GESCAMNAPPUER_003</t>
+  </si>
+  <si>
+    <t>Seleccionar un puerto y realizar el cambio</t>
+  </si>
+  <si>
+    <t>El usuario debe haber seleccionado una nap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Seleccionar puerto disponible
+2. Diligenciar el campo "ID DEAL"
+3. Diligenciar el campo "Comentario"
+4.Clic en el botón "Guardar"
+</t>
+  </si>
+  <si>
+    <t>El sistema debe haber seleccionado una nap y realizar el cambio</t>
+  </si>
+  <si>
+    <t>se realizo el cambio de nap correctamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,14 +522,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -500,7 +545,7 @@
     <col min="12" max="12" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="60">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="137.25" customHeight="1">
+    <row r="2" spans="1:12" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -573,6 +618,82 @@
         <v>18</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>